<commit_message>
DOMA-3110 added unitType to meter readings export
</commit_message>
<xml_diff>
--- a/apps/condo/domains/meter/templates/MeterReadingsExportTemplate.xlsx
+++ b/apps/condo/domains/meter/templates/MeterReadingsExportTemplate.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
   <si>
     <t>{d.i18n.date}</t>
   </si>
@@ -19,13 +19,16 @@
     <t>{d.i18n.address}</t>
   </si>
   <si>
-    <t>{d.i18n.unit}</t>
+    <t>{d.i18n.unitName}</t>
+  </si>
+  <si>
+    <t>{d.i18n.unitType}</t>
   </si>
   <si>
     <t>{d.i18n.accountNumber}</t>
   </si>
   <si>
-    <t>{d.i18n.service}</t>
+    <t>{d.i18n.resource}</t>
   </si>
   <si>
     <t>{d.i18n.number}</t>
@@ -61,6 +64,9 @@
     <t>{d.meter[i].unitName}</t>
   </si>
   <si>
+    <t>{d.meter[I].unitType}</t>
+  </si>
+  <si>
     <t>{d.meter[i].accountNumber}</t>
   </si>
   <si>
@@ -98,6 +104,9 @@
   </si>
   <si>
     <t>{d.meter[i + 1].unitName}</t>
+  </si>
+  <si>
+    <t>{d.meter[i + 1].unitType}</t>
   </si>
   <si>
     <t>{d.meter[i + 1].accountNumber}</t>
@@ -154,15 +163,21 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -172,16 +187,103 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -191,14 +293,41 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -218,6 +347,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -369,9 +499,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -451,7 +581,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -479,10 +609,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -738,9 +868,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1028,7 +1158,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1056,10 +1186,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1313,14 +1443,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="13" width="8" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7891" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1719" style="1" customWidth="1"/>
+    <col min="3" max="4" width="22" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.3516" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1719" style="1" customWidth="1"/>
+    <col min="9" max="12" width="19.1719" style="1" customWidth="1"/>
+    <col min="13" max="13" width="23.1719" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.3516" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
@@ -1363,88 +1502,209 @@
       <c r="M1" t="s" s="2">
         <v>12</v>
       </c>
+      <c r="N1" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s" s="2">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="N2" t="s" s="2">
+        <v>27</v>
       </c>
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="M3" t="s" s="2">
-        <v>38</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="N3" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" ht="15.35" customHeight="1">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" ht="15.35" customHeight="1">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="8"/>
+    </row>
+    <row r="6" ht="15.35" customHeight="1">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="8"/>
+    </row>
+    <row r="7" ht="15.35" customHeight="1">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="8"/>
+    </row>
+    <row r="8" ht="15.35" customHeight="1">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="8"/>
+    </row>
+    <row r="9" ht="15.35" customHeight="1">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="8"/>
+    </row>
+    <row r="10" ht="15.35" customHeight="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>